<commit_message>
switch column order to cluster together rankings
</commit_message>
<xml_diff>
--- a/output/ppedata_export.xlsx
+++ b/output/ppedata_export.xlsx
@@ -390,34 +390,34 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>n95_percapita_rank</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>n95_bytotalcases_rank</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>n95_bycases100k_rank</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>n95_percapita</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>n95_percapita_rank</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>n95_bycases100k</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>n95_bytotalcases</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>n95_bytotalcases_rank</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>n95_bycases100k</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>n95_bycases100k_rank</t>
-        </is>
-      </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
           <t>ventilators_DELIVERED</t>
@@ -425,32 +425,32 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
+          <t>vent_percapita_rank</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>vent_bytotalcases_rank</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>vent_bycases100K_rank</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
           <t>vent_percapita</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>vent_percapita_rank</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>vent_bytotalcases</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>vent_bytotalcases_rank</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>vent_bycases100K</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>vent_bycases100K_rank</t>
         </is>
       </c>
     </row>
@@ -478,43 +478,43 @@
         <v>152412</v>
       </c>
       <c r="G2">
+        <v>36</v>
+      </c>
+      <c r="H2">
+        <v>29</v>
+      </c>
+      <c r="I2">
+        <v>25</v>
+      </c>
+      <c r="J2">
         <v>0.03188711677799778</v>
-      </c>
-      <c r="H2">
-        <v>36</v>
-      </c>
-      <c r="I2">
-        <v>52.90246442207567</v>
-      </c>
-      <c r="J2">
-        <v>29</v>
       </c>
       <c r="K2">
         <v>2540.2</v>
       </c>
       <c r="L2">
-        <v>25</v>
+        <v>52.90246442207567</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O2">
         <v>16</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q2">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R2">
         <v>0</v>
       </c>
       <c r="S2">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -541,43 +541,43 @@
         <v>74115</v>
       </c>
       <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>28</v>
+      </c>
+      <c r="J3">
         <v>0.1043533723535019</v>
-      </c>
-      <c r="H3">
-        <v>6</v>
-      </c>
-      <c r="I3">
-        <v>315.3829787234043</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
       </c>
       <c r="K3">
         <v>2245.909090909091</v>
       </c>
       <c r="L3">
-        <v>28</v>
+        <v>315.3829787234043</v>
       </c>
       <c r="M3">
         <v>60</v>
       </c>
       <c r="N3">
+        <v>4</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>9</v>
+      </c>
+      <c r="Q3">
         <v>8.44795566512867e-005</v>
       </c>
-      <c r="O3">
-        <v>4</v>
-      </c>
-      <c r="P3">
+      <c r="R3">
         <v>0.2553191489361702</v>
       </c>
-      <c r="Q3">
-        <v>1</v>
-      </c>
-      <c r="R3">
+      <c r="S3">
         <v>1.818181818181818</v>
-      </c>
-      <c r="S3">
-        <v>9</v>
       </c>
     </row>
     <row r="4">
@@ -604,43 +604,43 @@
         <v>183432</v>
       </c>
       <c r="G4">
+        <v>44</v>
+      </c>
+      <c r="H4">
+        <v>25</v>
+      </c>
+      <c r="I4">
+        <v>8</v>
+      </c>
+      <c r="J4">
         <v>0.02869704507982379</v>
-      </c>
-      <c r="H4">
-        <v>44</v>
-      </c>
-      <c r="I4">
-        <v>60.41897233201581</v>
-      </c>
-      <c r="J4">
-        <v>25</v>
       </c>
       <c r="K4">
         <v>3902.808510638298</v>
       </c>
       <c r="L4">
-        <v>8</v>
+        <v>60.41897233201581</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O4">
         <v>16</v>
       </c>
       <c r="P4">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q4">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R4">
         <v>0</v>
       </c>
       <c r="S4">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -667,43 +667,43 @@
         <v>116552</v>
       </c>
       <c r="G5">
+        <v>26</v>
+      </c>
+      <c r="H5">
+        <v>17</v>
+      </c>
+      <c r="I5">
+        <v>19</v>
+      </c>
+      <c r="J5">
         <v>0.03997094568502956</v>
-      </c>
-      <c r="H5">
-        <v>26</v>
-      </c>
-      <c r="I5">
-        <v>100.1305841924399</v>
-      </c>
-      <c r="J5">
-        <v>17</v>
       </c>
       <c r="K5">
         <v>2913.8</v>
       </c>
       <c r="L5">
-        <v>19</v>
+        <v>100.1305841924399</v>
       </c>
       <c r="M5">
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O5">
         <v>16</v>
       </c>
       <c r="P5">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q5">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R5">
         <v>0</v>
       </c>
       <c r="S5">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -730,43 +730,43 @@
         <v>837662</v>
       </c>
       <c r="G6">
+        <v>54</v>
+      </c>
+      <c r="H6">
+        <v>38</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
         <v>0.0224851825132343</v>
-      </c>
-      <c r="H6">
-        <v>54</v>
-      </c>
-      <c r="I6">
-        <v>41.42125302872967</v>
-      </c>
-      <c r="J6">
-        <v>38</v>
       </c>
       <c r="K6">
         <v>15512.25925925926</v>
       </c>
       <c r="L6">
-        <v>1</v>
+        <v>41.42125302872967</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O6">
         <v>16</v>
       </c>
       <c r="P6">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q6">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R6">
         <v>0</v>
       </c>
       <c r="S6">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -793,43 +793,43 @@
         <v>217661</v>
       </c>
       <c r="G7">
+        <v>22</v>
+      </c>
+      <c r="H7">
+        <v>39</v>
+      </c>
+      <c r="I7">
+        <v>33</v>
+      </c>
+      <c r="J7">
         <v>0.04327948244610073</v>
-      </c>
-      <c r="H7">
-        <v>22</v>
-      </c>
-      <c r="I7">
-        <v>35.09529184134151</v>
-      </c>
-      <c r="J7">
-        <v>39</v>
       </c>
       <c r="K7">
         <v>1769.60162601626</v>
       </c>
       <c r="L7">
-        <v>33</v>
+        <v>35.09529184134151</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
       <c r="N7">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O7">
         <v>16</v>
       </c>
       <c r="P7">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q7">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R7">
         <v>0</v>
       </c>
       <c r="S7">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -856,43 +856,43 @@
         <v>189665</v>
       </c>
       <c r="G8">
+        <v>17</v>
+      </c>
+      <c r="H8">
+        <v>48</v>
+      </c>
+      <c r="I8">
+        <v>48</v>
+      </c>
+      <c r="J8">
         <v>0.05306655079590733</v>
-      </c>
-      <c r="H8">
-        <v>17</v>
-      </c>
-      <c r="I8">
-        <v>19.3852207686018</v>
-      </c>
-      <c r="J8">
-        <v>48</v>
       </c>
       <c r="K8">
         <v>692.2080291970802</v>
       </c>
       <c r="L8">
-        <v>48</v>
+        <v>19.3852207686018</v>
       </c>
       <c r="M8">
         <v>50</v>
       </c>
       <c r="N8">
+        <v>14</v>
+      </c>
+      <c r="O8">
+        <v>15</v>
+      </c>
+      <c r="P8">
+        <v>15</v>
+      </c>
+      <c r="Q8">
         <v>1.398954756963787e-005</v>
       </c>
-      <c r="O8">
-        <v>14</v>
-      </c>
-      <c r="P8">
+      <c r="R8">
         <v>0.005110384300899428</v>
       </c>
-      <c r="Q8">
-        <v>15</v>
-      </c>
-      <c r="R8">
+      <c r="S8">
         <v>0.1824817518248175</v>
-      </c>
-      <c r="S8">
-        <v>15</v>
       </c>
     </row>
     <row r="9">
@@ -919,43 +919,43 @@
         <v>77434</v>
       </c>
       <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="H9">
+        <v>23</v>
+      </c>
+      <c r="I9">
+        <v>51</v>
+      </c>
+      <c r="J9">
         <v>0.08623573670225206</v>
-      </c>
-      <c r="H9">
-        <v>8</v>
-      </c>
-      <c r="I9">
-        <v>64.04797353184451</v>
-      </c>
-      <c r="J9">
-        <v>23</v>
       </c>
       <c r="K9">
         <v>573.5851851851852</v>
       </c>
       <c r="L9">
-        <v>51</v>
+        <v>64.04797353184451</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
       <c r="N9">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O9">
         <v>16</v>
       </c>
       <c r="P9">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q9">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R9">
         <v>0</v>
       </c>
       <c r="S9">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -982,43 +982,43 @@
         <v>482635</v>
       </c>
       <c r="G10">
+        <v>48</v>
+      </c>
+      <c r="H10">
+        <v>43</v>
+      </c>
+      <c r="I10">
+        <v>6</v>
+      </c>
+      <c r="J10">
         <v>0.02567028574072764</v>
-      </c>
-      <c r="H10">
-        <v>48</v>
-      </c>
-      <c r="I10">
-        <v>27.53037476470253</v>
-      </c>
-      <c r="J10">
-        <v>43</v>
       </c>
       <c r="K10">
         <v>5189.623655913979</v>
       </c>
       <c r="L10">
-        <v>6</v>
+        <v>27.53037476470253</v>
       </c>
       <c r="M10">
         <v>200</v>
       </c>
       <c r="N10">
+        <v>15</v>
+      </c>
+      <c r="O10">
+        <v>13</v>
+      </c>
+      <c r="P10">
+        <v>6</v>
+      </c>
+      <c r="Q10">
         <v>1.063755663834063e-005</v>
       </c>
-      <c r="O10">
-        <v>15</v>
-      </c>
-      <c r="P10">
+      <c r="R10">
         <v>0.01140836232958759</v>
       </c>
-      <c r="Q10">
-        <v>13</v>
-      </c>
-      <c r="R10">
+      <c r="S10">
         <v>2.150537634408602</v>
-      </c>
-      <c r="S10">
-        <v>6</v>
       </c>
     </row>
     <row r="11">
@@ -1045,43 +1045,43 @@
         <v>307289</v>
       </c>
       <c r="G11">
+        <v>37</v>
+      </c>
+      <c r="H11">
+        <v>42</v>
+      </c>
+      <c r="I11">
+        <v>23</v>
+      </c>
+      <c r="J11">
         <v>0.03171965387282141</v>
-      </c>
-      <c r="H11">
-        <v>37</v>
-      </c>
-      <c r="I11">
-        <v>28.23050068902159</v>
-      </c>
-      <c r="J11">
-        <v>42</v>
       </c>
       <c r="K11">
         <v>2743.651785714286</v>
       </c>
       <c r="L11">
-        <v>23</v>
+        <v>28.23050068902159</v>
       </c>
       <c r="M11">
         <v>150</v>
       </c>
       <c r="N11">
+        <v>13</v>
+      </c>
+      <c r="O11">
+        <v>12</v>
+      </c>
+      <c r="P11">
+        <v>11</v>
+      </c>
+      <c r="Q11">
         <v>1.548362642633876e-005</v>
       </c>
-      <c r="O11">
-        <v>13</v>
-      </c>
-      <c r="P11">
+      <c r="R11">
         <v>0.01378043178686266</v>
       </c>
-      <c r="Q11">
-        <v>12</v>
-      </c>
-      <c r="R11">
+      <c r="S11">
         <v>1.339285714285714</v>
-      </c>
-      <c r="S11">
-        <v>11</v>
       </c>
     </row>
     <row r="12">
@@ -1108,43 +1108,43 @@
         <v>86622</v>
       </c>
       <c r="G12">
+        <v>15</v>
+      </c>
+      <c r="H12">
+        <v>5</v>
+      </c>
+      <c r="I12">
+        <v>24</v>
+      </c>
+      <c r="J12">
         <v>0.06367855349661582</v>
-      </c>
-      <c r="H12">
-        <v>15</v>
-      </c>
-      <c r="I12">
-        <v>195.9773755656109</v>
-      </c>
-      <c r="J12">
-        <v>5</v>
       </c>
       <c r="K12">
         <v>2706.9375</v>
       </c>
       <c r="L12">
-        <v>24</v>
+        <v>195.9773755656109</v>
       </c>
       <c r="M12">
         <v>0</v>
       </c>
       <c r="N12">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O12">
         <v>16</v>
       </c>
       <c r="P12">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q12">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R12">
         <v>0</v>
       </c>
       <c r="S12">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -1171,43 +1171,43 @@
         <v>90610</v>
       </c>
       <c r="G13">
+        <v>16</v>
+      </c>
+      <c r="H13">
+        <v>22</v>
+      </c>
+      <c r="I13">
+        <v>45</v>
+      </c>
+      <c r="J13">
         <v>0.05780239885377607</v>
-      </c>
-      <c r="H13">
-        <v>16</v>
-      </c>
-      <c r="I13">
-        <v>66.92023633677991</v>
-      </c>
-      <c r="J13">
-        <v>22</v>
       </c>
       <c r="K13">
         <v>1053.604651162791</v>
       </c>
       <c r="L13">
-        <v>45</v>
+        <v>66.92023633677991</v>
       </c>
       <c r="M13">
         <v>0</v>
       </c>
       <c r="N13">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O13">
         <v>16</v>
       </c>
       <c r="P13">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q13">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R13">
         <v>0</v>
       </c>
       <c r="S13">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -1234,43 +1234,43 @@
         <v>367760</v>
       </c>
       <c r="G14">
+        <v>45</v>
+      </c>
+      <c r="H14">
+        <v>46</v>
+      </c>
+      <c r="I14">
+        <v>21</v>
+      </c>
+      <c r="J14">
         <v>0.02866265667973331</v>
-      </c>
-      <c r="H14">
-        <v>45</v>
-      </c>
-      <c r="I14">
-        <v>22.39162201656113</v>
-      </c>
-      <c r="J14">
-        <v>46</v>
       </c>
       <c r="K14">
         <v>2873.125</v>
       </c>
       <c r="L14">
-        <v>21</v>
+        <v>22.39162201656113</v>
       </c>
       <c r="M14">
         <v>300</v>
       </c>
       <c r="N14">
+        <v>10</v>
+      </c>
+      <c r="O14">
+        <v>9</v>
+      </c>
+      <c r="P14">
+        <v>4</v>
+      </c>
+      <c r="Q14">
         <v>2.338154504002609e-005</v>
       </c>
-      <c r="O14">
-        <v>10</v>
-      </c>
-      <c r="P14">
+      <c r="R14">
         <v>0.01826595226497808</v>
       </c>
-      <c r="Q14">
-        <v>9</v>
-      </c>
-      <c r="R14">
+      <c r="S14">
         <v>2.34375</v>
-      </c>
-      <c r="S14">
-        <v>4</v>
       </c>
     </row>
     <row r="15">
@@ -1297,43 +1297,43 @@
         <v>185198</v>
       </c>
       <c r="G15">
+        <v>46</v>
+      </c>
+      <c r="H15">
+        <v>44</v>
+      </c>
+      <c r="I15">
+        <v>34</v>
+      </c>
+      <c r="J15">
         <v>0.02856317944317239</v>
-      </c>
-      <c r="H15">
-        <v>46</v>
-      </c>
-      <c r="I15">
-        <v>26.8130881714203</v>
-      </c>
-      <c r="J15">
-        <v>44</v>
       </c>
       <c r="K15">
         <v>1730.822429906542</v>
       </c>
       <c r="L15">
-        <v>34</v>
+        <v>26.8130881714203</v>
       </c>
       <c r="M15">
         <v>0</v>
       </c>
       <c r="N15">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O15">
         <v>16</v>
       </c>
       <c r="P15">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q15">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R15">
         <v>0</v>
       </c>
       <c r="S15">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -1360,43 +1360,43 @@
         <v>119062</v>
       </c>
       <c r="G16">
+        <v>28</v>
+      </c>
+      <c r="H16">
+        <v>19</v>
+      </c>
+      <c r="I16">
+        <v>22</v>
+      </c>
+      <c r="J16">
         <v>0.03908342921294465</v>
-      </c>
-      <c r="H16">
-        <v>28</v>
-      </c>
-      <c r="I16">
-        <v>93.7496062992126</v>
-      </c>
-      <c r="J16">
-        <v>19</v>
       </c>
       <c r="K16">
         <v>2834.809523809524</v>
       </c>
       <c r="L16">
-        <v>22</v>
+        <v>93.7496062992126</v>
       </c>
       <c r="M16">
         <v>0</v>
       </c>
       <c r="N16">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O16">
         <v>16</v>
       </c>
       <c r="P16">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q16">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R16">
         <v>0</v>
       </c>
       <c r="S16">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -1423,43 +1423,43 @@
         <v>115344</v>
       </c>
       <c r="G17">
+        <v>25</v>
+      </c>
+      <c r="H17">
+        <v>14</v>
+      </c>
+      <c r="I17">
+        <v>17</v>
+      </c>
+      <c r="J17">
         <v>0.04042735000795621</v>
-      </c>
-      <c r="H17">
-        <v>25</v>
-      </c>
-      <c r="I17">
-        <v>103.2623097582811</v>
-      </c>
-      <c r="J17">
-        <v>14</v>
       </c>
       <c r="K17">
         <v>2957.538461538461</v>
       </c>
       <c r="L17">
-        <v>17</v>
+        <v>103.2623097582811</v>
       </c>
       <c r="M17">
         <v>0</v>
       </c>
       <c r="N17">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O17">
         <v>16</v>
       </c>
       <c r="P17">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q17">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R17">
         <v>0</v>
       </c>
       <c r="S17">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -1486,43 +1486,43 @@
         <v>143939</v>
       </c>
       <c r="G18">
+        <v>33</v>
+      </c>
+      <c r="H18">
+        <v>18</v>
+      </c>
+      <c r="I18">
+        <v>7</v>
+      </c>
+      <c r="J18">
         <v>0.03317050620516771</v>
-      </c>
-      <c r="H18">
-        <v>33</v>
-      </c>
-      <c r="I18">
-        <v>99.13154269972452</v>
-      </c>
-      <c r="J18">
-        <v>18</v>
       </c>
       <c r="K18">
         <v>4361.787878787879</v>
       </c>
       <c r="L18">
-        <v>7</v>
+        <v>99.13154269972452</v>
       </c>
       <c r="M18">
         <v>0</v>
       </c>
       <c r="N18">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O18">
         <v>16</v>
       </c>
       <c r="P18">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q18">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R18">
         <v>0</v>
       </c>
       <c r="S18">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -1549,43 +1549,43 @@
         <v>208122</v>
       </c>
       <c r="G19">
+        <v>21</v>
+      </c>
+      <c r="H19">
+        <v>51</v>
+      </c>
+      <c r="I19">
+        <v>52</v>
+      </c>
+      <c r="J19">
         <v>0.04590887313019977</v>
-      </c>
-      <c r="H19">
-        <v>21</v>
-      </c>
-      <c r="I19">
-        <v>11.38336159273642</v>
-      </c>
-      <c r="J19">
-        <v>51</v>
       </c>
       <c r="K19">
         <v>516.4317617866005</v>
       </c>
       <c r="L19">
-        <v>52</v>
+        <v>11.38336159273642</v>
       </c>
       <c r="M19">
         <v>150</v>
       </c>
       <c r="N19">
+        <v>9</v>
+      </c>
+      <c r="O19">
+        <v>14</v>
+      </c>
+      <c r="P19">
+        <v>14</v>
+      </c>
+      <c r="Q19">
         <v>3.308795307334144e-005</v>
       </c>
-      <c r="O19">
-        <v>9</v>
-      </c>
-      <c r="P19">
+      <c r="R19">
         <v>0.008204342832139146</v>
       </c>
-      <c r="Q19">
-        <v>14</v>
-      </c>
-      <c r="R19">
+      <c r="S19">
         <v>0.3722084367245658</v>
-      </c>
-      <c r="S19">
-        <v>14</v>
       </c>
     </row>
     <row r="20">
@@ -1612,43 +1612,43 @@
         <v>86008</v>
       </c>
       <c r="G20">
+        <v>13</v>
+      </c>
+      <c r="H20">
+        <v>10</v>
+      </c>
+      <c r="I20">
+        <v>31</v>
+      </c>
+      <c r="J20">
         <v>0.06474745946320315</v>
-      </c>
-      <c r="H20">
-        <v>13</v>
-      </c>
-      <c r="I20">
-        <v>153.5857142857143</v>
-      </c>
-      <c r="J20">
-        <v>10</v>
       </c>
       <c r="K20">
         <v>2047.809523809524</v>
       </c>
       <c r="L20">
-        <v>31</v>
+        <v>153.5857142857143</v>
       </c>
       <c r="M20">
         <v>0</v>
       </c>
       <c r="N20">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O20">
         <v>16</v>
       </c>
       <c r="P20">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q20">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R20">
         <v>0</v>
       </c>
       <c r="S20">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -1675,43 +1675,43 @@
         <v>171533</v>
       </c>
       <c r="G21">
+        <v>41</v>
+      </c>
+      <c r="H21">
+        <v>45</v>
+      </c>
+      <c r="I21">
+        <v>38</v>
+      </c>
+      <c r="J21">
         <v>0.02971013338062947</v>
-      </c>
-      <c r="H21">
-        <v>41</v>
-      </c>
-      <c r="I21">
-        <v>24.61725028702641</v>
-      </c>
-      <c r="J21">
-        <v>45</v>
       </c>
       <c r="K21">
         <v>1417.628099173554</v>
       </c>
       <c r="L21">
-        <v>38</v>
+        <v>24.61725028702641</v>
       </c>
       <c r="M21">
         <v>120</v>
       </c>
       <c r="N21">
+        <v>11</v>
+      </c>
+      <c r="O21">
+        <v>10</v>
+      </c>
+      <c r="P21">
+        <v>12</v>
+      </c>
+      <c r="Q21">
         <v>2.078443218316904e-005</v>
       </c>
-      <c r="O21">
-        <v>11</v>
-      </c>
-      <c r="P21">
+      <c r="R21">
         <v>0.01722158438576349</v>
       </c>
-      <c r="Q21">
-        <v>10</v>
-      </c>
-      <c r="R21">
+      <c r="S21">
         <v>0.9917355371900827</v>
-      </c>
-      <c r="S21">
-        <v>12</v>
       </c>
     </row>
     <row r="22">
@@ -1738,43 +1738,43 @@
         <v>246876</v>
       </c>
       <c r="G22">
+        <v>30</v>
+      </c>
+      <c r="H22">
+        <v>50</v>
+      </c>
+      <c r="I22">
+        <v>46</v>
+      </c>
+      <c r="J22">
         <v>0.03770464087076406</v>
-      </c>
-      <c r="H22">
-        <v>30</v>
-      </c>
-      <c r="I22">
-        <v>13.0339475212502</v>
-      </c>
-      <c r="J22">
-        <v>50</v>
       </c>
       <c r="K22">
         <v>854.242214532872</v>
       </c>
       <c r="L22">
-        <v>46</v>
+        <v>13.0339475212502</v>
       </c>
       <c r="M22">
         <v>0</v>
       </c>
       <c r="N22">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O22">
         <v>16</v>
       </c>
       <c r="P22">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q22">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R22">
         <v>0</v>
       </c>
       <c r="S22">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -1801,43 +1801,43 @@
         <v>311060</v>
       </c>
       <c r="G23">
+        <v>38</v>
+      </c>
+      <c r="H23">
+        <v>49</v>
+      </c>
+      <c r="I23">
+        <v>37</v>
+      </c>
+      <c r="J23">
         <v>0.03147221064304244</v>
-      </c>
-      <c r="H23">
-        <v>38</v>
-      </c>
-      <c r="I23">
-        <v>14.46521577380952</v>
-      </c>
-      <c r="J23">
-        <v>49</v>
       </c>
       <c r="K23">
         <v>1426.880733944954</v>
       </c>
       <c r="L23">
-        <v>37</v>
+        <v>14.46521577380952</v>
       </c>
       <c r="M23">
         <v>400</v>
       </c>
       <c r="N23">
+        <v>7</v>
+      </c>
+      <c r="O23">
+        <v>8</v>
+      </c>
+      <c r="P23">
+        <v>8</v>
+      </c>
+      <c r="Q23">
         <v>4.047091962070654e-005</v>
       </c>
-      <c r="O23">
-        <v>7</v>
-      </c>
-      <c r="P23">
+      <c r="R23">
         <v>0.01860119047619048</v>
       </c>
-      <c r="Q23">
-        <v>8</v>
-      </c>
-      <c r="R23">
+      <c r="S23">
         <v>1.834862385321101</v>
-      </c>
-      <c r="S23">
-        <v>8</v>
       </c>
     </row>
     <row r="24">
@@ -1864,43 +1864,43 @@
         <v>162497</v>
       </c>
       <c r="G24">
+        <v>39</v>
+      </c>
+      <c r="H24">
+        <v>11</v>
+      </c>
+      <c r="I24">
+        <v>3</v>
+      </c>
+      <c r="J24">
         <v>0.0306371225083311</v>
-      </c>
-      <c r="H24">
-        <v>39</v>
-      </c>
-      <c r="I24">
-        <v>130.8349436392915</v>
-      </c>
-      <c r="J24">
-        <v>11</v>
       </c>
       <c r="K24">
         <v>7065.086956521739</v>
       </c>
       <c r="L24">
-        <v>3</v>
+        <v>130.8349436392915</v>
       </c>
       <c r="M24">
         <v>0</v>
       </c>
       <c r="N24">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O24">
         <v>16</v>
       </c>
       <c r="P24">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q24">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R24">
         <v>0</v>
       </c>
       <c r="S24">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1927,43 +1927,43 @@
         <v>117541</v>
       </c>
       <c r="G25">
+        <v>27</v>
+      </c>
+      <c r="H25">
+        <v>35</v>
+      </c>
+      <c r="I25">
+        <v>39</v>
+      </c>
+      <c r="J25">
         <v>0.03961214532957099</v>
-      </c>
-      <c r="H25">
-        <v>27</v>
-      </c>
-      <c r="I25">
-        <v>47.60672336978534</v>
-      </c>
-      <c r="J25">
-        <v>35</v>
       </c>
       <c r="K25">
         <v>1416.156626506024</v>
       </c>
       <c r="L25">
-        <v>39</v>
+        <v>47.60672336978534</v>
       </c>
       <c r="M25">
         <v>0</v>
       </c>
       <c r="N25">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O25">
         <v>16</v>
       </c>
       <c r="P25">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q25">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R25">
         <v>0</v>
       </c>
       <c r="S25">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -1990,43 +1990,43 @@
         <v>175676</v>
       </c>
       <c r="G26">
+        <v>42</v>
+      </c>
+      <c r="H26">
+        <v>34</v>
+      </c>
+      <c r="I26">
+        <v>20</v>
+      </c>
+      <c r="J26">
         <v>0.02933346824898684</v>
-      </c>
-      <c r="H26">
-        <v>42</v>
-      </c>
-      <c r="I26">
-        <v>48.4757174392936</v>
-      </c>
-      <c r="J26">
-        <v>34</v>
       </c>
       <c r="K26">
         <v>2879.934426229508</v>
       </c>
       <c r="L26">
-        <v>20</v>
+        <v>48.4757174392936</v>
       </c>
       <c r="M26">
         <v>0</v>
       </c>
       <c r="N26">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O26">
         <v>16</v>
       </c>
       <c r="P26">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q26">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R26">
         <v>0</v>
       </c>
       <c r="S26">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -2053,43 +2053,43 @@
         <v>79486</v>
       </c>
       <c r="G27">
+        <v>9</v>
+      </c>
+      <c r="H27">
+        <v>4</v>
+      </c>
+      <c r="I27">
+        <v>29</v>
+      </c>
+      <c r="J27">
         <v>0.08033636037456476</v>
-      </c>
-      <c r="H27">
-        <v>9</v>
-      </c>
-      <c r="I27">
-        <v>224.5367231638418</v>
-      </c>
-      <c r="J27">
-        <v>4</v>
       </c>
       <c r="K27">
         <v>2207.944444444444</v>
       </c>
       <c r="L27">
-        <v>29</v>
+        <v>224.5367231638418</v>
       </c>
       <c r="M27">
         <v>0</v>
       </c>
       <c r="N27">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O27">
         <v>16</v>
       </c>
       <c r="P27">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q27">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R27">
         <v>0</v>
       </c>
       <c r="S27">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -2116,43 +2116,43 @@
         <v>95589</v>
       </c>
       <c r="G28">
+        <v>18</v>
+      </c>
+      <c r="H28">
+        <v>9</v>
+      </c>
+      <c r="I28">
+        <v>16</v>
+      </c>
+      <c r="J28">
         <v>0.0523390757804813</v>
-      </c>
-      <c r="H28">
-        <v>18</v>
-      </c>
-      <c r="I28">
-        <v>165.6655112651646</v>
-      </c>
-      <c r="J28">
-        <v>9</v>
       </c>
       <c r="K28">
         <v>2987.15625</v>
       </c>
       <c r="L28">
-        <v>16</v>
+        <v>165.6655112651646</v>
       </c>
       <c r="M28">
         <v>0</v>
       </c>
       <c r="N28">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O28">
         <v>16</v>
       </c>
       <c r="P28">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q28">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R28">
         <v>0</v>
       </c>
       <c r="S28">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -2179,43 +2179,43 @@
         <v>112408</v>
       </c>
       <c r="G29">
+        <v>23</v>
+      </c>
+      <c r="H29">
+        <v>37</v>
+      </c>
+      <c r="I29">
+        <v>43</v>
+      </c>
+      <c r="J29">
         <v>0.04162409819329463</v>
-      </c>
-      <c r="H29">
-        <v>23</v>
-      </c>
-      <c r="I29">
-        <v>45.08945046129162</v>
-      </c>
-      <c r="J29">
-        <v>37</v>
       </c>
       <c r="K29">
         <v>1221.826086956522</v>
       </c>
       <c r="L29">
-        <v>43</v>
+        <v>45.08945046129162</v>
       </c>
       <c r="M29">
         <v>0</v>
       </c>
       <c r="N29">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O29">
         <v>16</v>
       </c>
       <c r="P29">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q29">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R29">
         <v>0</v>
       </c>
       <c r="S29">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -2242,43 +2242,43 @@
         <v>85779</v>
       </c>
       <c r="G30">
+        <v>12</v>
+      </c>
+      <c r="H30">
+        <v>13</v>
+      </c>
+      <c r="I30">
+        <v>41</v>
+      </c>
+      <c r="J30">
         <v>0.06515834010649692</v>
-      </c>
-      <c r="H30">
-        <v>12</v>
-      </c>
-      <c r="I30">
-        <v>104.7362637362637</v>
-      </c>
-      <c r="J30">
-        <v>13</v>
       </c>
       <c r="K30">
         <v>1383.532258064516</v>
       </c>
       <c r="L30">
-        <v>41</v>
+        <v>104.7362637362637</v>
       </c>
       <c r="M30">
         <v>0</v>
       </c>
       <c r="N30">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O30">
         <v>16</v>
       </c>
       <c r="P30">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q30">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R30">
         <v>0</v>
       </c>
       <c r="S30">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -2305,43 +2305,43 @@
         <v>290055</v>
       </c>
       <c r="G31">
+        <v>34</v>
+      </c>
+      <c r="H31">
+        <v>53</v>
+      </c>
+      <c r="I31">
+        <v>54</v>
+      </c>
+      <c r="J31">
         <v>0.03299118483457603</v>
-      </c>
-      <c r="H31">
-        <v>34</v>
-      </c>
-      <c r="I31">
-        <v>5.313530446251924</v>
-      </c>
-      <c r="J31">
-        <v>53</v>
       </c>
       <c r="K31">
         <v>467.0772946859904</v>
       </c>
       <c r="L31">
-        <v>54</v>
+        <v>5.313530446251924</v>
       </c>
       <c r="M31">
         <v>1100</v>
       </c>
       <c r="N31">
+        <v>2</v>
+      </c>
+      <c r="O31">
+        <v>7</v>
+      </c>
+      <c r="P31">
+        <v>10</v>
+      </c>
+      <c r="Q31">
         <v>0.0001251152482047668</v>
       </c>
-      <c r="O31">
-        <v>2</v>
-      </c>
-      <c r="P31">
+      <c r="R31">
         <v>0.02015094892650399</v>
       </c>
-      <c r="Q31">
-        <v>7</v>
-      </c>
-      <c r="R31">
+      <c r="S31">
         <v>1.77133655394525</v>
-      </c>
-      <c r="S31">
-        <v>10</v>
       </c>
     </row>
     <row r="32">
@@ -2368,43 +2368,43 @@
         <v>100068</v>
       </c>
       <c r="G32">
+        <v>20</v>
+      </c>
+      <c r="H32">
+        <v>16</v>
+      </c>
+      <c r="I32">
+        <v>30</v>
+      </c>
+      <c r="J32">
         <v>0.04859606668482924</v>
-      </c>
-      <c r="H32">
-        <v>20</v>
-      </c>
-      <c r="I32">
-        <v>101.1809908998989</v>
-      </c>
-      <c r="J32">
-        <v>16</v>
       </c>
       <c r="K32">
         <v>2084.75</v>
       </c>
       <c r="L32">
-        <v>30</v>
+        <v>101.1809908998989</v>
       </c>
       <c r="M32">
         <v>0</v>
       </c>
       <c r="N32">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O32">
         <v>16</v>
       </c>
       <c r="P32">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q32">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R32">
         <v>0</v>
       </c>
       <c r="S32">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -2431,43 +2431,43 @@
         <v>493733</v>
       </c>
       <c r="G33">
+        <v>50</v>
+      </c>
+      <c r="H33">
+        <v>54</v>
+      </c>
+      <c r="I33">
+        <v>50</v>
+      </c>
+      <c r="J33">
         <v>0.0254789142920189</v>
-      </c>
-      <c r="H33">
-        <v>50</v>
-      </c>
-      <c r="I33">
-        <v>3.051369841848622</v>
-      </c>
-      <c r="J33">
-        <v>54</v>
       </c>
       <c r="K33">
         <v>591.2970059880239</v>
       </c>
       <c r="L33">
-        <v>50</v>
+        <v>3.051369841848622</v>
       </c>
       <c r="M33">
         <v>2400</v>
       </c>
       <c r="N33">
+        <v>3</v>
+      </c>
+      <c r="O33">
+        <v>11</v>
+      </c>
+      <c r="P33">
+        <v>3</v>
+      </c>
+      <c r="Q33">
         <v>0.0001238511387750978</v>
       </c>
-      <c r="O33">
-        <v>3</v>
-      </c>
-      <c r="P33">
+      <c r="R33">
         <v>0.01483248561557905</v>
       </c>
-      <c r="Q33">
-        <v>11</v>
-      </c>
-      <c r="R33">
+      <c r="S33">
         <v>2.874251497005988</v>
-      </c>
-      <c r="S33">
-        <v>3</v>
       </c>
     </row>
     <row r="34">
@@ -2494,43 +2494,43 @@
         <v>243912</v>
       </c>
       <c r="G34">
+        <v>49</v>
+      </c>
+      <c r="H34">
+        <v>24</v>
+      </c>
+      <c r="I34">
+        <v>5</v>
+      </c>
+      <c r="J34">
         <v>0.02557940693722594</v>
-      </c>
-      <c r="H34">
-        <v>49</v>
-      </c>
-      <c r="I34">
-        <v>61.56284704694599</v>
-      </c>
-      <c r="J34">
-        <v>24</v>
       </c>
       <c r="K34">
         <v>5807.428571428572</v>
       </c>
       <c r="L34">
-        <v>5</v>
+        <v>61.56284704694599</v>
       </c>
       <c r="M34">
         <v>0</v>
       </c>
       <c r="N34">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O34">
         <v>16</v>
       </c>
       <c r="P34">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q34">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R34">
         <v>0</v>
       </c>
       <c r="S34">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -2557,43 +2557,43 @@
         <v>73391</v>
       </c>
       <c r="G35">
+        <v>5</v>
+      </c>
+      <c r="H35">
+        <v>3</v>
+      </c>
+      <c r="I35">
+        <v>32</v>
+      </c>
+      <c r="J35">
         <v>0.1091168332612241</v>
-      </c>
-      <c r="H35">
-        <v>5</v>
-      </c>
-      <c r="I35">
-        <v>272.8289962825279</v>
-      </c>
-      <c r="J35">
-        <v>3</v>
       </c>
       <c r="K35">
         <v>1834.775</v>
       </c>
       <c r="L35">
-        <v>32</v>
+        <v>272.8289962825279</v>
       </c>
       <c r="M35">
         <v>0</v>
       </c>
       <c r="N35">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O35">
         <v>16</v>
       </c>
       <c r="P35">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q35">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R35">
         <v>0</v>
       </c>
       <c r="S35">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -2620,43 +2620,43 @@
         <v>282411</v>
       </c>
       <c r="G36">
+        <v>52</v>
+      </c>
+      <c r="H36">
+        <v>32</v>
+      </c>
+      <c r="I36">
+        <v>4</v>
+      </c>
+      <c r="J36">
         <v>0.02447977307510144</v>
-      </c>
-      <c r="H36">
-        <v>52</v>
-      </c>
-      <c r="I36">
-        <v>51.23566763425254</v>
-      </c>
-      <c r="J36">
-        <v>32</v>
       </c>
       <c r="K36">
         <v>5883.5625</v>
       </c>
       <c r="L36">
-        <v>4</v>
+        <v>51.23566763425254</v>
       </c>
       <c r="M36">
         <v>0</v>
       </c>
       <c r="N36">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O36">
         <v>16</v>
       </c>
       <c r="P36">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q36">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R36">
         <v>0</v>
       </c>
       <c r="S36">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -2683,43 +2683,43 @@
         <v>132626</v>
       </c>
       <c r="G37">
+        <v>31</v>
+      </c>
+      <c r="H37">
+        <v>21</v>
+      </c>
+      <c r="I37">
+        <v>18</v>
+      </c>
+      <c r="J37">
         <v>0.03535419639484549</v>
-      </c>
-      <c r="H37">
-        <v>31</v>
-      </c>
-      <c r="I37">
-        <v>78.66310794780546</v>
-      </c>
-      <c r="J37">
-        <v>21</v>
       </c>
       <c r="K37">
         <v>2947.244444444445</v>
       </c>
       <c r="L37">
-        <v>18</v>
+        <v>78.66310794780546</v>
       </c>
       <c r="M37">
         <v>0</v>
       </c>
       <c r="N37">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O37">
         <v>16</v>
       </c>
       <c r="P37">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q37">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R37">
         <v>0</v>
       </c>
       <c r="S37">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -2746,43 +2746,43 @@
         <v>134159</v>
       </c>
       <c r="G38">
+        <v>32</v>
+      </c>
+      <c r="H38">
+        <v>15</v>
+      </c>
+      <c r="I38">
+        <v>9</v>
+      </c>
+      <c r="J38">
         <v>0.03501863968171849</v>
-      </c>
-      <c r="H38">
-        <v>32</v>
-      </c>
-      <c r="I38">
-        <v>101.481845688351</v>
-      </c>
-      <c r="J38">
-        <v>15</v>
       </c>
       <c r="K38">
         <v>3833.114285714286</v>
       </c>
       <c r="L38">
-        <v>9</v>
+        <v>101.481845688351</v>
       </c>
       <c r="M38">
         <v>140</v>
       </c>
       <c r="N38">
+        <v>8</v>
+      </c>
+      <c r="O38">
+        <v>2</v>
+      </c>
+      <c r="P38">
+        <v>1</v>
+      </c>
+      <c r="Q38">
         <v>3.654327742037872e-005</v>
       </c>
-      <c r="O38">
-        <v>8</v>
-      </c>
-      <c r="P38">
+      <c r="R38">
         <v>0.1059001512859304</v>
       </c>
-      <c r="Q38">
-        <v>2</v>
-      </c>
-      <c r="R38">
+      <c r="S38">
         <v>4</v>
-      </c>
-      <c r="S38">
-        <v>1</v>
       </c>
     </row>
     <row r="39">
@@ -2809,43 +2809,43 @@
         <v>365293</v>
       </c>
       <c r="G39">
+        <v>43</v>
+      </c>
+      <c r="H39">
+        <v>47</v>
+      </c>
+      <c r="I39">
+        <v>27</v>
+      </c>
+      <c r="J39">
         <v>0.02875784134609745</v>
-      </c>
-      <c r="H39">
-        <v>43</v>
-      </c>
-      <c r="I39">
-        <v>19.60462620082649</v>
-      </c>
-      <c r="J39">
-        <v>47</v>
       </c>
       <c r="K39">
         <v>2484.986394557823</v>
       </c>
       <c r="L39">
-        <v>27</v>
+        <v>19.60462620082649</v>
       </c>
       <c r="M39">
         <v>0</v>
       </c>
       <c r="N39">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O39">
         <v>16</v>
       </c>
       <c r="P39">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q39">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R39">
         <v>0</v>
       </c>
       <c r="S39">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -2872,43 +2872,43 @@
         <v>213486</v>
       </c>
       <c r="G40">
+        <v>3</v>
+      </c>
+      <c r="H40">
+        <v>12</v>
+      </c>
+      <c r="I40">
+        <v>42</v>
+      </c>
+      <c r="J40">
         <v>0.2028241432611891</v>
-      </c>
-      <c r="H40">
-        <v>3</v>
-      </c>
-      <c r="I40">
-        <v>123.6166763173133</v>
-      </c>
-      <c r="J40">
-        <v>12</v>
       </c>
       <c r="K40">
         <v>1301.743902439024</v>
       </c>
       <c r="L40">
-        <v>42</v>
+        <v>123.6166763173133</v>
       </c>
       <c r="M40">
         <v>0</v>
       </c>
       <c r="N40">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O40">
         <v>16</v>
       </c>
       <c r="P40">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q40">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R40">
         <v>0</v>
       </c>
       <c r="S40">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -2935,43 +2935,43 @@
         <v>149442</v>
       </c>
       <c r="G41">
+        <v>35</v>
+      </c>
+      <c r="H41">
+        <v>28</v>
+      </c>
+      <c r="I41">
+        <v>26</v>
+      </c>
+      <c r="J41">
         <v>0.03230924095919802</v>
-      </c>
-      <c r="H41">
-        <v>35</v>
-      </c>
-      <c r="I41">
-        <v>53.50590762620838</v>
-      </c>
-      <c r="J41">
-        <v>28</v>
       </c>
       <c r="K41">
         <v>2490.7</v>
       </c>
       <c r="L41">
-        <v>26</v>
+        <v>53.50590762620838</v>
       </c>
       <c r="M41">
         <v>0</v>
       </c>
       <c r="N41">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O41">
         <v>16</v>
       </c>
       <c r="P41">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q41">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R41">
         <v>0</v>
       </c>
       <c r="S41">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -2998,43 +2998,43 @@
         <v>76115</v>
       </c>
       <c r="G42">
+        <v>7</v>
+      </c>
+      <c r="H42">
+        <v>8</v>
+      </c>
+      <c r="I42">
+        <v>40</v>
+      </c>
+      <c r="J42">
         <v>0.09348669827310914</v>
-      </c>
-      <c r="H42">
-        <v>7</v>
-      </c>
-      <c r="I42">
-        <v>170.2796420581655</v>
-      </c>
-      <c r="J42">
-        <v>8</v>
       </c>
       <c r="K42">
         <v>1383.909090909091</v>
       </c>
       <c r="L42">
-        <v>40</v>
+        <v>170.2796420581655</v>
       </c>
       <c r="M42">
         <v>0</v>
       </c>
       <c r="N42">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O42">
         <v>16</v>
       </c>
       <c r="P42">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q42">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R42">
         <v>0</v>
       </c>
       <c r="S42">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -3061,43 +3061,43 @@
         <v>242998</v>
       </c>
       <c r="G43">
+        <v>29</v>
+      </c>
+      <c r="H43">
+        <v>31</v>
+      </c>
+      <c r="I43">
+        <v>13</v>
+      </c>
+      <c r="J43">
         <v>0.03829088866320365</v>
-      </c>
-      <c r="H43">
-        <v>29</v>
-      </c>
-      <c r="I43">
-        <v>52.4380664652568</v>
-      </c>
-      <c r="J43">
-        <v>31</v>
       </c>
       <c r="K43">
         <v>3328.739726027397</v>
       </c>
       <c r="L43">
-        <v>13</v>
+        <v>52.4380664652568</v>
       </c>
       <c r="M43">
         <v>0</v>
       </c>
       <c r="N43">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O43">
         <v>16</v>
       </c>
       <c r="P43">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q43">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R43">
         <v>0</v>
       </c>
       <c r="S43">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -3124,43 +3124,43 @@
         <v>604698</v>
       </c>
       <c r="G44">
+        <v>53</v>
+      </c>
+      <c r="H44">
+        <v>30</v>
+      </c>
+      <c r="I44">
+        <v>2</v>
+      </c>
+      <c r="J44">
         <v>0.02404790253039095</v>
-      </c>
-      <c r="H44">
-        <v>53</v>
-      </c>
-      <c r="I44">
-        <v>52.66028041452582</v>
-      </c>
-      <c r="J44">
-        <v>30</v>
       </c>
       <c r="K44">
         <v>13145.60869565217</v>
       </c>
       <c r="L44">
-        <v>2</v>
+        <v>52.66028041452582</v>
       </c>
       <c r="M44">
         <v>0</v>
       </c>
       <c r="N44">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O44">
         <v>16</v>
       </c>
       <c r="P44">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q44">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R44">
         <v>0</v>
       </c>
       <c r="S44">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -3187,43 +3187,43 @@
         <v>113627</v>
       </c>
       <c r="G45">
+        <v>24</v>
+      </c>
+      <c r="H45">
+        <v>27</v>
+      </c>
+      <c r="I45">
+        <v>36</v>
+      </c>
+      <c r="J45">
         <v>0.04111133422700293</v>
-      </c>
-      <c r="H45">
-        <v>24</v>
-      </c>
-      <c r="I45">
-        <v>57.47445624683864</v>
-      </c>
-      <c r="J45">
-        <v>27</v>
       </c>
       <c r="K45">
         <v>1578.152777777778</v>
       </c>
       <c r="L45">
-        <v>36</v>
+        <v>57.47445624683864</v>
       </c>
       <c r="M45">
         <v>0</v>
       </c>
       <c r="N45">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O45">
         <v>16</v>
       </c>
       <c r="P45">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q45">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R45">
         <v>0</v>
       </c>
       <c r="S45">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -3250,43 +3250,43 @@
         <v>132939</v>
       </c>
       <c r="G46">
+        <v>2</v>
+      </c>
+      <c r="H46">
+        <v>6</v>
+      </c>
+      <c r="I46">
+        <v>44</v>
+      </c>
+      <c r="J46">
         <v>0.2124505186650707</v>
-      </c>
-      <c r="H46">
-        <v>2</v>
-      </c>
-      <c r="I46">
-        <v>195.7864506627393</v>
-      </c>
-      <c r="J46">
-        <v>6</v>
       </c>
       <c r="K46">
         <v>1219.623853211009</v>
       </c>
       <c r="L46">
-        <v>44</v>
+        <v>195.7864506627393</v>
       </c>
       <c r="M46">
         <v>0</v>
       </c>
       <c r="N46">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O46">
         <v>16</v>
       </c>
       <c r="P46">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q46">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R46">
         <v>0</v>
       </c>
       <c r="S46">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -3313,43 +3313,43 @@
         <v>214389</v>
       </c>
       <c r="G47">
+        <v>47</v>
+      </c>
+      <c r="H47">
+        <v>36</v>
+      </c>
+      <c r="I47">
+        <v>10</v>
+      </c>
+      <c r="J47">
         <v>0.02679519521501248</v>
-      </c>
-      <c r="H47">
-        <v>47</v>
-      </c>
-      <c r="I47">
-        <v>47.54690618762475</v>
-      </c>
-      <c r="J47">
-        <v>36</v>
       </c>
       <c r="K47">
         <v>3828.375</v>
       </c>
       <c r="L47">
-        <v>10</v>
+        <v>47.54690618762475</v>
       </c>
       <c r="M47">
         <v>0</v>
       </c>
       <c r="N47">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O47">
         <v>16</v>
       </c>
       <c r="P47">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q47">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R47">
         <v>0</v>
       </c>
       <c r="S47">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -3376,43 +3376,43 @@
         <v>489959</v>
       </c>
       <c r="G48">
+        <v>11</v>
+      </c>
+      <c r="H48">
+        <v>33</v>
+      </c>
+      <c r="I48">
+        <v>11</v>
+      </c>
+      <c r="J48">
         <v>0.07286134070137139</v>
-      </c>
-      <c r="H48">
-        <v>11</v>
-      </c>
-      <c r="I48">
-        <v>50.23674766738439</v>
-      </c>
-      <c r="J48">
-        <v>33</v>
       </c>
       <c r="K48">
         <v>3379.027586206897</v>
       </c>
       <c r="L48">
-        <v>11</v>
+        <v>50.23674766738439</v>
       </c>
       <c r="M48">
         <v>500</v>
       </c>
       <c r="N48">
+        <v>5</v>
+      </c>
+      <c r="O48">
+        <v>3</v>
+      </c>
+      <c r="P48">
+        <v>2</v>
+      </c>
+      <c r="Q48">
         <v>7.435452833948493e-005</v>
       </c>
-      <c r="O48">
-        <v>5</v>
-      </c>
-      <c r="P48">
+      <c r="R48">
         <v>0.05126627704296114</v>
       </c>
-      <c r="Q48">
-        <v>3</v>
-      </c>
-      <c r="R48">
+      <c r="S48">
         <v>3.448275862068965</v>
-      </c>
-      <c r="S48">
-        <v>2</v>
       </c>
     </row>
     <row r="49">
@@ -3439,43 +3439,43 @@
         <v>96101</v>
       </c>
       <c r="G49">
+        <v>19</v>
+      </c>
+      <c r="H49">
+        <v>7</v>
+      </c>
+      <c r="I49">
+        <v>14</v>
+      </c>
+      <c r="J49">
         <v>0.05186255325165651</v>
-      </c>
-      <c r="H49">
-        <v>19</v>
-      </c>
-      <c r="I49">
-        <v>179.2929104477612</v>
-      </c>
-      <c r="J49">
-        <v>7</v>
       </c>
       <c r="K49">
         <v>3313.827586206897</v>
       </c>
       <c r="L49">
-        <v>14</v>
+        <v>179.2929104477612</v>
       </c>
       <c r="M49">
         <v>0</v>
       </c>
       <c r="N49">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O49">
         <v>16</v>
       </c>
       <c r="P49">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q49">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R49">
         <v>0</v>
       </c>
       <c r="S49">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -3502,43 +3502,43 @@
         <v>169867</v>
       </c>
       <c r="G50">
+        <v>40</v>
+      </c>
+      <c r="H50">
+        <v>26</v>
+      </c>
+      <c r="I50">
+        <v>12</v>
+      </c>
+      <c r="J50">
         <v>0.02986942468295157</v>
-      </c>
-      <c r="H50">
-        <v>40</v>
-      </c>
-      <c r="I50">
-        <v>58.77750865051903</v>
-      </c>
-      <c r="J50">
-        <v>26</v>
       </c>
       <c r="K50">
         <v>3330.725490196078</v>
       </c>
       <c r="L50">
-        <v>12</v>
+        <v>58.77750865051903</v>
       </c>
       <c r="M50">
         <v>0</v>
       </c>
       <c r="N50">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O50">
         <v>16</v>
       </c>
       <c r="P50">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q50">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R50">
         <v>0</v>
       </c>
       <c r="S50">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -3565,43 +3565,43 @@
         <v>71294</v>
       </c>
       <c r="G51">
+        <v>4</v>
+      </c>
+      <c r="H51">
+        <v>2</v>
+      </c>
+      <c r="I51">
+        <v>35</v>
+      </c>
+      <c r="J51">
         <v>0.126491680653483</v>
-      </c>
-      <c r="H51">
-        <v>4</v>
-      </c>
-      <c r="I51">
-        <v>298.3012552301256</v>
-      </c>
-      <c r="J51">
-        <v>2</v>
       </c>
       <c r="K51">
         <v>1697.47619047619</v>
       </c>
       <c r="L51">
-        <v>35</v>
+        <v>298.3012552301256</v>
       </c>
       <c r="M51">
         <v>0</v>
       </c>
       <c r="N51">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O51">
         <v>16</v>
       </c>
       <c r="P51">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q51">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R51">
         <v>0</v>
       </c>
       <c r="S51">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -3628,43 +3628,43 @@
         <v>132477</v>
       </c>
       <c r="G52">
+        <v>1</v>
+      </c>
+      <c r="H52">
+        <v>20</v>
+      </c>
+      <c r="I52">
+        <v>53</v>
+      </c>
+      <c r="J52">
         <v>0.2201627659238553</v>
-      </c>
-      <c r="H52">
-        <v>1</v>
-      </c>
-      <c r="I52">
-        <v>79.80542168674698</v>
-      </c>
-      <c r="J52">
-        <v>20</v>
       </c>
       <c r="K52">
         <v>479.9891304347826</v>
       </c>
       <c r="L52">
-        <v>53</v>
+        <v>79.80542168674698</v>
       </c>
       <c r="M52">
         <v>0</v>
       </c>
       <c r="N52">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O52">
         <v>16</v>
       </c>
       <c r="P52">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q52">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R52">
         <v>0</v>
       </c>
       <c r="S52">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -3691,43 +3691,43 @@
         <v>172763</v>
       </c>
       <c r="G53">
+        <v>14</v>
+      </c>
+      <c r="H53">
+        <v>41</v>
+      </c>
+      <c r="I53">
+        <v>47</v>
+      </c>
+      <c r="J53">
         <v>0.06409078801809469</v>
-      </c>
-      <c r="H53">
-        <v>14</v>
-      </c>
-      <c r="I53">
-        <v>28.32644695851779</v>
-      </c>
-      <c r="J53">
-        <v>41</v>
       </c>
       <c r="K53">
         <v>764.4380530973451</v>
       </c>
       <c r="L53">
-        <v>47</v>
+        <v>28.32644695851779</v>
       </c>
       <c r="M53">
         <v>150</v>
       </c>
       <c r="N53">
+        <v>6</v>
+      </c>
+      <c r="O53">
+        <v>5</v>
+      </c>
+      <c r="P53">
+        <v>13</v>
+      </c>
+      <c r="Q53">
         <v>5.564627960103844e-005</v>
       </c>
-      <c r="O53">
-        <v>6</v>
-      </c>
-      <c r="P53">
+      <c r="R53">
         <v>0.02459419576979833</v>
       </c>
-      <c r="Q53">
-        <v>5</v>
-      </c>
-      <c r="R53">
+      <c r="S53">
         <v>0.6637168141592921</v>
-      </c>
-      <c r="S53">
-        <v>13</v>
       </c>
     </row>
     <row r="54">
@@ -3754,43 +3754,43 @@
         <v>249359</v>
       </c>
       <c r="G54">
+        <v>51</v>
+      </c>
+      <c r="H54">
+        <v>40</v>
+      </c>
+      <c r="I54">
+        <v>15</v>
+      </c>
+      <c r="J54">
         <v>0.02539658128624178</v>
-      </c>
-      <c r="H54">
-        <v>51</v>
-      </c>
-      <c r="I54">
-        <v>33.11540504648075</v>
-      </c>
-      <c r="J54">
-        <v>40</v>
       </c>
       <c r="K54">
         <v>3238.428571428572</v>
       </c>
       <c r="L54">
-        <v>15</v>
+        <v>33.11540504648075</v>
       </c>
       <c r="M54">
         <v>170</v>
       </c>
       <c r="N54">
+        <v>12</v>
+      </c>
+      <c r="O54">
+        <v>6</v>
+      </c>
+      <c r="P54">
+        <v>5</v>
+      </c>
+      <c r="Q54">
         <v>1.731406854639738e-005</v>
       </c>
-      <c r="O54">
-        <v>12</v>
-      </c>
-      <c r="P54">
+      <c r="R54">
         <v>0.02257636122177955</v>
       </c>
-      <c r="Q54">
-        <v>6</v>
-      </c>
-      <c r="R54">
+      <c r="S54">
         <v>2.207792207792208</v>
-      </c>
-      <c r="S54">
-        <v>5</v>
       </c>
     </row>
     <row r="55">
@@ -3817,43 +3817,43 @@
         <v>603189</v>
       </c>
       <c r="G55">
+        <v>10</v>
+      </c>
+      <c r="H55">
+        <v>52</v>
+      </c>
+      <c r="I55">
+        <v>49</v>
+      </c>
+      <c r="J55">
         <v>0.07378338676569543</v>
-      </c>
-      <c r="H55">
-        <v>10</v>
-      </c>
-      <c r="I55">
-        <v>7.520684753877612</v>
-      </c>
-      <c r="J55">
-        <v>52</v>
       </c>
       <c r="K55">
         <v>614.8715596330276</v>
       </c>
       <c r="L55">
-        <v>49</v>
+        <v>7.520684753877612</v>
       </c>
       <c r="M55">
         <v>2000</v>
       </c>
       <c r="N55">
+        <v>1</v>
+      </c>
+      <c r="O55">
+        <v>4</v>
+      </c>
+      <c r="P55">
+        <v>7</v>
+      </c>
+      <c r="Q55">
         <v>0.0002446443378963988</v>
       </c>
-      <c r="O55">
-        <v>1</v>
-      </c>
-      <c r="P55">
+      <c r="R55">
         <v>0.02493641214902</v>
       </c>
-      <c r="Q55">
-        <v>4</v>
-      </c>
-      <c r="R55">
+      <c r="S55">
         <v>2.038735983690112</v>
-      </c>
-      <c r="S55">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>